<commit_message>
Update Test Case documentation
</commit_message>
<xml_diff>
--- a/Documentation/QA_documentation.xlsx
+++ b/Documentation/QA_documentation.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Famouscave\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Famouscave\Documents\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41C1048-0DEF-4DC4-BBB1-F723CAB5DD0C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D6F133-EBA6-4AE6-815D-28102A50507E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{81C84C01-0F36-4DC8-A114-6D8E54D90FBD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{81C84C01-0F36-4DC8-A114-6D8E54D90FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="backend" sheetId="1" r:id="rId1"/>
-    <sheet name="frontend" sheetId="2" r:id="rId2"/>
+    <sheet name="design" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="105">
   <si>
     <t>Test Case #1</t>
   </si>
@@ -73,21 +73,9 @@
     <t>Tested the Main menu buttons</t>
   </si>
   <si>
-    <t>Choose option Begin</t>
-  </si>
-  <si>
-    <t>Choose option Rules</t>
-  </si>
-  <si>
     <t>Choose option Quit</t>
   </si>
   <si>
-    <t>Start a game</t>
-  </si>
-  <si>
-    <t>Open rules</t>
-  </si>
-  <si>
     <t>Close the programme</t>
   </si>
   <si>
@@ -181,12 +169,6 @@
     <t>Designed card sprites</t>
   </si>
   <si>
-    <t>Design button "Rules"</t>
-  </si>
-  <si>
-    <t>Design button "Begin"</t>
-  </si>
-  <si>
     <t>Design button "Quit"</t>
   </si>
   <si>
@@ -299,6 +281,66 @@
   </si>
   <si>
     <t>13th May</t>
+  </si>
+  <si>
+    <t>Press "escape" key to go back to main menu</t>
+  </si>
+  <si>
+    <t>Returns player back to main menu</t>
+  </si>
+  <si>
+    <t>Start with 5 cards</t>
+  </si>
+  <si>
+    <t>Start the game with each player having 5 cards at the start</t>
+  </si>
+  <si>
+    <t>Placing cards you selected on the table</t>
+  </si>
+  <si>
+    <t>Skipping player's turn and drawing a card</t>
+  </si>
+  <si>
+    <t>Press "Discard" button</t>
+  </si>
+  <si>
+    <t>Choose option PVP</t>
+  </si>
+  <si>
+    <t>Choose option PVC</t>
+  </si>
+  <si>
+    <t>Starts a game Player vs Computer</t>
+  </si>
+  <si>
+    <t>Start a game Player vs Player on local PC</t>
+  </si>
+  <si>
+    <t>Game ending with player 1 winning the game</t>
+  </si>
+  <si>
+    <t>Game ending with player 2 winning the game</t>
+  </si>
+  <si>
+    <t>Design button PVP</t>
+  </si>
+  <si>
+    <t>Design button PVC</t>
+  </si>
+  <si>
+    <t>Main menu extras</t>
+  </si>
+  <si>
+    <t>Design game icon</t>
+  </si>
+  <si>
+    <t>14th May</t>
+  </si>
+  <si>
+    <t>Designed Main menu icon and background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design Main menu background </t>
   </si>
 </sst>
 </file>
@@ -800,16 +842,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC9A78-089F-4084-9E60-78E63F8CF698}">
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M86" sqref="M86"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="4" max="5" width="35.140625" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
@@ -863,7 +904,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -892,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>6</v>
@@ -907,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -915,22 +956,22 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>18</v>
+        <v>92</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I11" s="8">
         <v>1</v>
@@ -940,23 +981,23 @@
       <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>16</v>
+      <c r="C12" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="I12" s="8">
         <v>2</v>
@@ -967,31 +1008,69 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I13" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>27</v>
-      </c>
+    <row r="14" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -1002,167 +1081,169 @@
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+    </row>
     <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G25" s="4">
         <v>44690</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+    <row r="26" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D28" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>25</v>
+      <c r="E29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I30" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="F31" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I31" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
-        <v>3</v>
-      </c>
-      <c r="C32" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>35</v>
-      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -1173,167 +1254,169 @@
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="18"/>
+    </row>
     <row r="43" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18"/>
+      <c r="D43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G44" s="4">
         <v>44690</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:10" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+    <row r="45" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="6" t="s">
+      <c r="D47" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I48" s="6" t="s">
-        <v>25</v>
+      <c r="I47" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="7">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I48" s="8">
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I49" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I50" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
-        <v>3</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I51" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>60</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+    </row>
+    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
@@ -1344,141 +1427,143 @@
       <c r="I58" s="19"/>
       <c r="J58" s="19"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="18"/>
+    </row>
     <row r="62" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="18"/>
-    </row>
-    <row r="63" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>61</v>
+        <v>3</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="F63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="4">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="7">
+        <v>1</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I67" s="8">
         <v>11</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="4">
-        <v>44690</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>41</v>
+        <v>91</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I68" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="7">
-        <v>2</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I69" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
-        <v>67</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+    </row>
+    <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="19"/>
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
@@ -1489,167 +1574,194 @@
       <c r="I76" s="19"/>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
-      <c r="J77" s="19"/>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="18"/>
+    </row>
     <row r="80" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="18"/>
+      <c r="D80" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="81" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D81" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E81" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" s="4">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="7">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" s="2" t="s">
+      <c r="E85" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I85" s="8">
         <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G82" s="4">
-        <v>44690</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C86" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D86" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="E86" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H86" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I86" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G87" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H87" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I87" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D88" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="I88" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E88" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G88" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H88" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I88" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
-        <v>84</v>
-      </c>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
+      <c r="J94" s="19"/>
+    </row>
+    <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="19"/>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
@@ -1660,151 +1772,141 @@
       <c r="I95" s="19"/>
       <c r="J95" s="19"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="19"/>
-      <c r="B96" s="19"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="19"/>
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
-      <c r="J96" s="19"/>
-    </row>
-    <row r="98" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D98" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="18"/>
+    </row>
     <row r="99" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D99" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="18"/>
+      <c r="D99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="100" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D100" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>81</v>
+        <v>3</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="101" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D101" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F101" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G101" s="4">
+      <c r="G100" s="4">
         <v>44690</v>
       </c>
     </row>
-    <row r="102" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="6" t="s">
+    <row r="101" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G101" s="1"/>
+    </row>
+    <row r="102" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E104" s="6" t="s">
+      <c r="D103" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E103" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F104" s="6" t="s">
+      <c r="F103" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G104" s="6" t="s">
+      <c r="G103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H104" s="6" t="s">
+      <c r="H103" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I104" s="6" t="s">
-        <v>25</v>
+      <c r="I103" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B104" s="7">
+        <v>1</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I104" s="8">
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E105" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H105" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D105" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G105" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H105" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="I105" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="7">
-        <v>2</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F106" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H106" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I106" s="8">
-        <v>16</v>
-      </c>
-    </row>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="A57:J58"/>
+    <mergeCell ref="D42:G42"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A20:J21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="A39:J40"/>
-    <mergeCell ref="D99:G99"/>
-    <mergeCell ref="A58:J59"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="A76:J77"/>
-    <mergeCell ref="D80:G80"/>
-    <mergeCell ref="A95:J96"/>
+    <mergeCell ref="A19:J20"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="A38:J39"/>
+    <mergeCell ref="D98:G98"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="A75:J76"/>
+    <mergeCell ref="D79:G79"/>
+    <mergeCell ref="A94:J95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1813,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0260D82F-FBBF-410F-BF2C-CCD0E955AFB2}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,13 +1975,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1887,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
@@ -1920,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1928,19 +2030,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H11" s="8">
         <v>1</v>
@@ -1951,19 +2053,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H12" s="8">
         <v>2</v>
@@ -1974,19 +2076,19 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13" s="8">
         <v>3</v>
@@ -1997,7 +2099,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -2035,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>11</v>
@@ -2049,7 +2151,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>10</v>
@@ -2082,7 +2184,7 @@
         <v>9</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2090,19 +2192,19 @@
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H30" s="8">
         <v>4</v>
@@ -2113,19 +2215,19 @@
         <v>2</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H31" s="8">
         <v>5</v>
@@ -2136,19 +2238,19 @@
         <v>3</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H32" s="8">
         <v>6</v>
@@ -2159,19 +2261,19 @@
         <v>4</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H33" s="8">
         <v>7</v>
@@ -2182,19 +2284,19 @@
         <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H34" s="8">
         <v>8</v>
@@ -2205,19 +2307,19 @@
         <v>6</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H35" s="8">
         <v>9</v>
@@ -2225,7 +2327,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -2263,7 +2365,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>11</v>
@@ -2277,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>10</v>
@@ -2310,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -2318,19 +2420,19 @@
         <v>1</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H52" s="8">
         <v>10</v>
@@ -2341,19 +2443,19 @@
         <v>2</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H53" s="8">
         <v>11</v>
@@ -2361,7 +2463,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
@@ -2394,12 +2496,12 @@
       <c r="F64" s="17"/>
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="2:8" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D65" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>11</v>
@@ -2408,12 +2510,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>10</v>
@@ -2422,11 +2524,11 @@
         <v>44690</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
         <v>1</v>
       </c>
@@ -2446,57 +2548,195 @@
         <v>9</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
         <v>1</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H70" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="7">
         <v>2</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H71" s="8">
         <v>12</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+    </row>
+    <row r="81" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+    </row>
+    <row r="83" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D83" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D84" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="4">
+        <v>44690</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="7">
+        <v>1</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H88" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="7">
+        <v>2</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H89" s="8">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A78:J79"/>
+    <mergeCell ref="D82:G82"/>
     <mergeCell ref="A42:J43"/>
     <mergeCell ref="D46:G46"/>
     <mergeCell ref="A60:J61"/>

</xml_diff>